<commit_message>
update della tabella di marcia
</commit_message>
<xml_diff>
--- a/Elenco attività per i progetti1.xlsx
+++ b/Elenco attività per i progetti1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giacomo\OneDrive - ISTITUTO D'ISTRUZIONE SUPERIORE JEAN MONNET\Documenti\GitHub\20220113_gestioneprogetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riccardo\Desktop\SCUOLA\Garden-Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8B349A-5373-46E6-8D5A-67F61E95C5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Progetto 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <definedName name="TitoloColonna2">Progetto2[[#Headers],[% completamento]]</definedName>
     <definedName name="TitoloColonna3">Progetto3[[#Headers],[% completamento]]</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <webPublishing codePage="1252"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -143,7 +142,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -408,7 +407,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Data" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Data" xfId="6"/>
     <cellStyle name="Normale" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percentuale" xfId="5" builtinId="5"/>
     <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -673,7 +672,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Elenco attività per i progetti">
-    <tableStyle name="Elenco attività per i progetti" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Elenco attività per i progetti" pivot="0" count="7">
       <tableStyleElement type="wholeTable" dxfId="19"/>
       <tableStyleElement type="headerRow" dxfId="18"/>
       <tableStyleElement type="totalRow" dxfId="17"/>
@@ -695,13 +694,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Progetto1" displayName="Progetto1" ref="B7:E17" totalsRowShown="0">
-  <autoFilter ref="B7:E17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Progetto1" displayName="Progetto1" ref="B7:E17" totalsRowShown="0">
+  <autoFilter ref="B7:E17"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="% completamento"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fase"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Scadenza" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Note"/>
+    <tableColumn id="1" name="% completamento"/>
+    <tableColumn id="2" name="Fase"/>
+    <tableColumn id="3" name="Scadenza" dataDxfId="12"/>
+    <tableColumn id="4" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="Elenco attività per i progetti" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -713,13 +712,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Progetto2" displayName="Progetto2" ref="B7:E16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B7:E16" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Progetto2" displayName="Progetto2" ref="B7:E16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="B7:E16"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="% completamento" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Fase" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Scadenza" dataDxfId="7" dataCellStyle="Data"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Note" dataDxfId="6"/>
+    <tableColumn id="1" name="% completamento" dataDxfId="9"/>
+    <tableColumn id="2" name="Fase" dataDxfId="8"/>
+    <tableColumn id="3" name="Scadenza" dataDxfId="7" dataCellStyle="Data"/>
+    <tableColumn id="4" name="Note" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Elenco attività per i progetti" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -731,13 +730,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Progetto3" displayName="Progetto3" ref="B7:E16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="B7:E16" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Progetto3" displayName="Progetto3" ref="B7:E16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="B7:E16"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="% completamento" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Fase" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Scadenza" dataDxfId="1" dataCellStyle="Data"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Note" dataDxfId="0"/>
+    <tableColumn id="1" name="% completamento" dataDxfId="3"/>
+    <tableColumn id="2" name="Fase" dataDxfId="2"/>
+    <tableColumn id="3" name="Scadenza" dataDxfId="1" dataCellStyle="Data"/>
+    <tableColumn id="4" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Elenco attività per i progetti" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1091,29 +1090,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.75" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="30.75" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.625" customWidth="1"/>
-    <col min="6" max="6" width="2.75" customWidth="1"/>
-    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="16"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -1122,8 +1121,8 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
@@ -1131,7 +1130,7 @@
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="22" t="s">
         <v>2</v>
       </c>
@@ -1141,8 +1140,8 @@
       </c>
       <c r="E4" s="21"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
@@ -1150,7 +1149,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
@@ -1164,7 +1163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12">
         <v>1</v>
       </c>
@@ -1178,7 +1177,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>1</v>
       </c>
@@ -1192,7 +1191,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12">
         <v>1</v>
       </c>
@@ -1206,7 +1205,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>0.75</v>
       </c>
@@ -1220,9 +1219,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
@@ -1234,9 +1233,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -1248,7 +1247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="12">
         <v>0.25</v>
       </c>
@@ -1262,9 +1261,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -1276,7 +1275,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12">
         <v>0.1</v>
       </c>
@@ -1290,7 +1289,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="19"/>
     </row>
   </sheetData>
@@ -1311,17 +1310,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per i progetti in questa cartella di lavoro. Immettere i dettagli del Progetto 1 in questo foglio di lavoro e i dettagli del Progetto 2 e del Progetto 3 nei fogli di lavoro successivi" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 1 nella tabella sottostante" sqref="B6:E6" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento si aggiorna automaticamente in ogni riga. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per i progetti in questa cartella di lavoro. Immettere i dettagli del Progetto 1 in questo foglio di lavoro e i dettagli del Progetto 2 e del Progetto 3 nei fogli di lavoro successivi" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 1 nella tabella sottostante" sqref="B6:E6"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento si aggiorna automaticamente in ogni riga. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
@@ -1336,7 +1335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1345,18 +1344,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.75" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="30.75" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.625" customWidth="1"/>
-    <col min="6" max="6" width="2.75" customWidth="1"/>
-    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="16"/>
       <c r="B1" s="9" t="str">
         <f>Titolo</f>
@@ -1366,8 +1365,8 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
@@ -1377,7 +1376,7 @@
       </c>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="22" t="s">
         <v>2</v>
       </c>
@@ -1387,8 +1386,8 @@
       </c>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>19</v>
       </c>
@@ -1396,7 +1395,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -1410,7 +1409,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
         <v>0</v>
       </c>
@@ -1420,7 +1419,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14">
         <v>0</v>
       </c>
@@ -1430,7 +1429,7 @@
       <c r="D9" s="17"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>0</v>
       </c>
@@ -1440,7 +1439,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14">
         <v>0</v>
       </c>
@@ -1450,7 +1449,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14">
         <v>0</v>
       </c>
@@ -1460,7 +1459,7 @@
       <c r="D12" s="17"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14">
         <v>0</v>
       </c>
@@ -1470,7 +1469,7 @@
       <c r="D13" s="17"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14">
         <v>0</v>
       </c>
@@ -1480,7 +1479,7 @@
       <c r="D14" s="17"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14">
         <v>0</v>
       </c>
@@ -1490,7 +1489,7 @@
       <c r="D15" s="17"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="14">
         <v>0</v>
       </c>
@@ -1518,17 +1517,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 2 nella tabella sottostante" sqref="B6:E6" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento viene aggiornata automaticamente. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per il Progetto 2 in questo foglio di lavoro" sqref="A1" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1" xr:uid="{00000000-0002-0000-0100-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3" xr:uid="{00000000-0002-0000-0100-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3" xr:uid="{00000000-0002-0000-0100-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 2 nella tabella sottostante" sqref="B6:E6"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento viene aggiornata automaticamente. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per il Progetto 2 in questo foglio di lavoro" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
@@ -1543,7 +1542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1552,18 +1551,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.75" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="30.75" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.625" customWidth="1"/>
-    <col min="6" max="6" width="2.75" customWidth="1"/>
-    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="16"/>
       <c r="B1" s="9" t="str">
         <f>Titolo</f>
@@ -1573,8 +1572,8 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
@@ -1584,7 +1583,7 @@
       </c>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="22" t="s">
         <v>2</v>
       </c>
@@ -1594,8 +1593,8 @@
       </c>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>20</v>
       </c>
@@ -1603,7 +1602,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -1617,7 +1616,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
         <v>0</v>
       </c>
@@ -1627,7 +1626,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14">
         <v>0</v>
       </c>
@@ -1637,7 +1636,7 @@
       <c r="D9" s="17"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>0</v>
       </c>
@@ -1647,7 +1646,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14">
         <v>0</v>
       </c>
@@ -1657,7 +1656,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14">
         <v>0</v>
       </c>
@@ -1667,7 +1666,7 @@
       <c r="D12" s="17"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14">
         <v>0</v>
       </c>
@@ -1677,7 +1676,7 @@
       <c r="D13" s="17"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14">
         <v>0</v>
       </c>
@@ -1687,7 +1686,7 @@
       <c r="D14" s="17"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14">
         <v>0</v>
       </c>
@@ -1697,7 +1696,7 @@
       <c r="D15" s="17"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15">
         <v>0</v>
       </c>
@@ -1707,7 +1706,7 @@
       <c r="D16" s="17"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E17" s="16"/>
     </row>
   </sheetData>
@@ -1728,17 +1727,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per il Progetto 3 in questo foglio di lavoro" sqref="A1" xr:uid="{00000000-0002-0000-0200-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 3 nella tabella sottostante" sqref="B6:E6" xr:uid="{00000000-0002-0000-0200-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento viene aggiornata automaticamente. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7" xr:uid="{00000000-0002-0000-0200-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4" xr:uid="{00000000-0002-0000-0200-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4" xr:uid="{00000000-0002-0000-0200-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1" xr:uid="{00000000-0002-0000-0200-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3" xr:uid="{00000000-0002-0000-0200-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3" xr:uid="{00000000-0002-0000-0200-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per il Progetto 3 in questo foglio di lavoro" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 3 nella tabella sottostante" sqref="B6:E6"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento viene aggiornata automaticamente. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Update Elenco attività per i progetti1.xlsx
</commit_message>
<xml_diff>
--- a/Elenco attività per i progetti1.xlsx
+++ b/Elenco attività per i progetti1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riccardo\Desktop\SCUOLA\Garden-Planner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JMatter\Documents\GitHub\Garden-Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EAE0D3-3BB9-4FB0-B8E6-B5BE18321217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Progetto 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
     <definedName name="TitoloColonna2">Progetto2[[#Headers],[% completamento]]</definedName>
     <definedName name="TitoloColonna3">Progetto3[[#Headers],[% completamento]]</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <webPublishing codePage="1252"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -124,9 +125,6 @@
     <t>Camagni Riccardo &amp; Russo Edoardo</t>
   </si>
   <si>
-    <t>Grafica del sito</t>
-  </si>
-  <si>
     <t>Pianificazione Web Server</t>
   </si>
   <si>
@@ -137,12 +135,15 @@
   </si>
   <si>
     <t>Gestione connessione al DataBase</t>
+  </si>
+  <si>
+    <t>Grafica teorica del sito</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -407,7 +408,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Data" xfId="6"/>
+    <cellStyle name="Data" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normale" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percentuale" xfId="5" builtinId="5"/>
     <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -672,7 +673,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Elenco attività per i progetti">
-    <tableStyle name="Elenco attività per i progetti" pivot="0" count="7">
+    <tableStyle name="Elenco attività per i progetti" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="19"/>
       <tableStyleElement type="headerRow" dxfId="18"/>
       <tableStyleElement type="totalRow" dxfId="17"/>
@@ -694,13 +695,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Progetto1" displayName="Progetto1" ref="B7:E17" totalsRowShown="0">
-  <autoFilter ref="B7:E17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Progetto1" displayName="Progetto1" ref="B7:E17" totalsRowShown="0">
+  <autoFilter ref="B7:E17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="% completamento"/>
-    <tableColumn id="2" name="Fase"/>
-    <tableColumn id="3" name="Scadenza" dataDxfId="12"/>
-    <tableColumn id="4" name="Note"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="% completamento"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fase"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Scadenza" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="Elenco attività per i progetti" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -712,13 +713,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Progetto2" displayName="Progetto2" ref="B7:E16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B7:E16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Progetto2" displayName="Progetto2" ref="B7:E16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="B7:E16" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="% completamento" dataDxfId="9"/>
-    <tableColumn id="2" name="Fase" dataDxfId="8"/>
-    <tableColumn id="3" name="Scadenza" dataDxfId="7" dataCellStyle="Data"/>
-    <tableColumn id="4" name="Note" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="% completamento" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Fase" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Scadenza" dataDxfId="7" dataCellStyle="Data"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Note" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Elenco attività per i progetti" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -730,13 +731,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Progetto3" displayName="Progetto3" ref="B7:E16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="B7:E16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Progetto3" displayName="Progetto3" ref="B7:E16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="B7:E16" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="% completamento" dataDxfId="3"/>
-    <tableColumn id="2" name="Fase" dataDxfId="2"/>
-    <tableColumn id="3" name="Scadenza" dataDxfId="1" dataCellStyle="Data"/>
-    <tableColumn id="4" name="Note" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="% completamento" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Fase" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Scadenza" dataDxfId="1" dataCellStyle="Data"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Elenco attività per i progetti" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1090,7 +1091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1098,7 +1099,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1207,10 +1208,10 @@
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D11" s="18">
         <v>44672</v>
@@ -1224,7 +1225,7 @@
         <v>0.15</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="18">
         <v>44623</v>
@@ -1238,7 +1239,7 @@
         <v>0.35</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="18">
         <v>44672</v>
@@ -1249,10 +1250,10 @@
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="12">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="18">
         <v>44679</v>
@@ -1266,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="18">
         <v>44630</v>
@@ -1310,17 +1311,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per i progetti in questa cartella di lavoro. Immettere i dettagli del Progetto 1 in questo foglio di lavoro e i dettagli del Progetto 2 e del Progetto 3 nei fogli di lavoro successivi" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 1 nella tabella sottostante" sqref="B6:E6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento si aggiorna automaticamente in ogni riga. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per i progetti in questa cartella di lavoro. Immettere i dettagli del Progetto 1 in questo foglio di lavoro e i dettagli del Progetto 2 e del Progetto 3 nei fogli di lavoro successivi" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 1 nella tabella sottostante" sqref="B6:E6" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento si aggiorna automaticamente in ogni riga. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
@@ -1335,7 +1336,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1517,17 +1518,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 2 nella tabella sottostante" sqref="B6:E6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento viene aggiornata automaticamente. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per il Progetto 2 in questo foglio di lavoro" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 2 nella tabella sottostante" sqref="B6:E6" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento viene aggiornata automaticamente. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per il Progetto 2 in questo foglio di lavoro" sqref="A1" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1" xr:uid="{00000000-0002-0000-0100-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3" xr:uid="{00000000-0002-0000-0100-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3" xr:uid="{00000000-0002-0000-0100-00000A000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
@@ -1542,7 +1543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1727,17 +1728,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per il Progetto 3 in questo foglio di lavoro" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 3 nella tabella sottostante" sqref="B6:E6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento viene aggiornata automaticamente. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere le note in questa colonna sotto questa intestazione" sqref="E7" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa colonna sotto questa intestazione" sqref="D7" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la fase del progetto in questa colonna sotto questa intestazione" sqref="C7" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Creare un elenco di attività per il Progetto 3 in questo foglio di lavoro" sqref="A1" xr:uid="{00000000-0002-0000-0200-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere i dettagli del Progetto 3 nella tabella sottostante" sqref="B6:E6" xr:uid="{00000000-0002-0000-0200-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la percentuale di completamento in questa colonna sotto questa intestazione. La barra dei dati che mostra la percentuale di completamento viene aggiornata automaticamente. Usare i filtri delle intestazioni per trovare voci specifiche" sqref="B7" xr:uid="{00000000-0002-0000-0200-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza nella cella a destra" sqref="B4:C4" xr:uid="{00000000-0002-0000-0200-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la data di scadenza in questa cella" sqref="D4:E4" xr:uid="{00000000-0002-0000-0200-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Il titolo del foglio di lavoro si trova in questa cella. Immettere il nome dell'incaricato del completamento del progetto nella cella D3 e la data di scadenza nella cella D4. Immettere i dettagli del progetto nella tabella a partire dalla cella B7" sqref="B1" xr:uid="{00000000-0002-0000-0200-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento nella cella a destra" sqref="B3:C3" xr:uid="{00000000-0002-0000-0200-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'incaricato del completamento in questa cella" sqref="D3:E3" xr:uid="{00000000-0002-0000-0200-00000A000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>

</xml_diff>